<commit_message>
* Replace button with multi language
</commit_message>
<xml_diff>
--- a/trunk/Resources/language.xlsx
+++ b/trunk/Resources/language.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="113">
   <si>
     <t>Id</t>
   </si>
@@ -101,9 +101,6 @@
     <t>tut_content</t>
   </si>
   <si>
-    <t>tut_misson</t>
-  </si>
-  <si>
     <t>....1972 Cuộc tập kích của địch diễn ra liên tục nhiều ngày với trọng tâm là các cuộc ném bom của B-52 vào ban đêm....</t>
   </si>
   <si>
@@ -255,6 +252,117 @@
   </si>
   <si>
     <t>Liên kết Facebook để thêm bạn, thêm quà!</t>
+  </si>
+  <si>
+    <t>btn_ask_friend</t>
+  </si>
+  <si>
+    <t>Ask friend</t>
+  </si>
+  <si>
+    <t>Xin bạn</t>
+  </si>
+  <si>
+    <t>Cất cánh</t>
+  </si>
+  <si>
+    <t>Lift up</t>
+  </si>
+  <si>
+    <t>btn_start</t>
+  </si>
+  <si>
+    <t>btn_exit</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>Thoát</t>
+  </si>
+  <si>
+    <t>btn_revive</t>
+  </si>
+  <si>
+    <t>Revive</t>
+  </si>
+  <si>
+    <t>Hồi sinh</t>
+  </si>
+  <si>
+    <t>btn_end</t>
+  </si>
+  <si>
+    <t>End game</t>
+  </si>
+  <si>
+    <t>Kết thúc</t>
+  </si>
+  <si>
+    <t>btn_no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>btn_yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Có</t>
+  </si>
+  <si>
+    <t>btn_gift</t>
+  </si>
+  <si>
+    <t>Gift</t>
+  </si>
+  <si>
+    <t>Quà tặng</t>
+  </si>
+  <si>
+    <t>btn_restart</t>
+  </si>
+  <si>
+    <t>Restart</t>
+  </si>
+  <si>
+    <t>Chơi lại</t>
+  </si>
+  <si>
+    <t>btn_resume</t>
+  </si>
+  <si>
+    <t>Resume</t>
+  </si>
+  <si>
+    <t>Tiếp tục</t>
+  </si>
+  <si>
+    <t>btn_share</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>Chia sẻ</t>
+  </si>
+  <si>
+    <t>btn_leaderboard</t>
+  </si>
+  <si>
+    <t>Leaderboard</t>
+  </si>
+  <si>
+    <t>Xếp hạng</t>
+  </si>
+  <si>
+    <t>tut_mission</t>
   </si>
 </sst>
 </file>
@@ -277,7 +385,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +437,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF25FF88"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCDACE6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -413,6 +527,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,6 +536,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCDACE6"/>
+      <color rgb="FFB17ED8"/>
       <color rgb="FF25FF88"/>
       <color rgb="FF6CD4F4"/>
     </mruColors>
@@ -699,16 +816,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="47" style="1" customWidth="1"/>
-    <col min="2" max="2" width="124.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="92.5703125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -726,13 +843,13 @@
     </row>
     <row r="2" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>54</v>
-      </c>
       <c r="C2" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -776,7 +893,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -828,197 +945,329 @@
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>72</v>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Button : Multi language
</commit_message>
<xml_diff>
--- a/trunk/Resources/language.xlsx
+++ b/trunk/Resources/language.xlsx
@@ -95,9 +95,6 @@
     <t>feed_error_caption</t>
   </si>
   <si>
-    <t>Couldn't share</t>
-  </si>
-  <si>
     <t>tut_content</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>score_server_error</t>
   </si>
   <si>
-    <t>Can not connect to server</t>
-  </si>
-  <si>
     <t>Không thể kết nối máy chủ</t>
   </si>
   <si>
@@ -363,6 +357,12 @@
   </si>
   <si>
     <t>tut_mission</t>
+  </si>
+  <si>
+    <t>Could not connect to server</t>
+  </si>
+  <si>
+    <t>Could not share</t>
   </si>
 </sst>
 </file>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -843,13 +843,13 @@
     </row>
     <row r="2" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -893,7 +893,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -934,7 +934,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>112</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -942,332 +942,332 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="C25" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* rate with multi language
</commit_message>
<xml_diff>
--- a/trunk/Resources/language.xlsx
+++ b/trunk/Resources/language.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cocos2DX2\projects\PhiCongButChi\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="127">
   <si>
     <t>Id</t>
   </si>
@@ -53,27 +53,15 @@
     <t>feed_deep_link</t>
   </si>
   <si>
-    <t>I've got %d pts in Điện Biên Phủ trên không, follow me is %s. Kaka :v</t>
-  </si>
-  <si>
     <t>Ta vừa đạt %d điểm trong game Điện Biên Phủ trên không, vượt qua %s. Kaka :v</t>
   </si>
   <si>
     <t>Điện Biên Phủ trên không -- Game bắn máy bay hot nhất 2014</t>
   </si>
   <si>
-    <t>Điện Biên Phủ trên không -- the best space shooting game in 2014</t>
-  </si>
-  <si>
     <t>Thử thách cùng bạn bè</t>
   </si>
   <si>
-    <t>Dare your all friend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Live in the lagend of 12-days </t>
-  </si>
-  <si>
     <t>https://dl.dropboxusercontent.com/u/41829250/DienBienPhuTrenKhong/DienBienPhuTrenKhong.jpg</t>
   </si>
   <si>
@@ -101,24 +89,15 @@
     <t>....1972 Cuộc tập kích của địch diễn ra liên tục nhiều ngày với trọng tâm là các cuộc ném bom của B-52 vào ban đêm....</t>
   </si>
   <si>
-    <t>1972 .... The enemy ambush ongoing for several days with a focus on the B-52 bomber at night ....</t>
-  </si>
-  <si>
     <t>Không được để lọt lưới trên 3 chiếc B-52 !!!</t>
   </si>
   <si>
-    <t>Do not let more than 3 B-52 go over you !!!</t>
-  </si>
-  <si>
     <t>Score</t>
   </si>
   <si>
     <t>Điểm</t>
   </si>
   <si>
-    <t>You have not enough diamond!</t>
-  </si>
-  <si>
     <t>Bạn không đủ số kim cương!</t>
   </si>
   <si>
@@ -155,9 +134,6 @@
     <t>Bạn có muốn thoát game!</t>
   </si>
   <si>
-    <t>Do you want to exit!</t>
-  </si>
-  <si>
     <t>score_invite_to_facebook</t>
   </si>
   <si>
@@ -182,9 +158,6 @@
     <t>Điện Biên Phủ trên không</t>
   </si>
   <si>
-    <t>%s is fighting to kill enemies in Điện Biên Phủ trên không. Come in to help your friend now!</t>
-  </si>
-  <si>
     <t>score_limit_lazer</t>
   </si>
   <si>
@@ -227,12 +200,6 @@
     <t>wait_lack_of_life</t>
   </si>
   <si>
-    <t>You have no gift. Call your friends to get more every day!</t>
-  </si>
-  <si>
-    <t>You have not enough life. Please wait!</t>
-  </si>
-  <si>
     <t>Bạn không đủ số mạng. Hãy chờ thêm!</t>
   </si>
   <si>
@@ -242,27 +209,18 @@
     <t>Cùng sống lại những giây phút hào hùng của dân tộc trong chiến thắng vẻ vang của "12 ngày đêm". Thử thách cùng bạn bè, vượt lên bảng xếp hạng. Click ngay để tải!</t>
   </si>
   <si>
-    <t>Connect  facebook for more friend, more gift!</t>
-  </si>
-  <si>
     <t>Liên kết Facebook để thêm bạn, thêm quà!</t>
   </si>
   <si>
     <t>btn_ask_friend</t>
   </si>
   <si>
-    <t>Ask friend</t>
-  </si>
-  <si>
     <t>Xin bạn</t>
   </si>
   <si>
     <t>Cất cánh</t>
   </si>
   <si>
-    <t>Lift up</t>
-  </si>
-  <si>
     <t>btn_start</t>
   </si>
   <si>
@@ -350,19 +308,103 @@
     <t>btn_leaderboard</t>
   </si>
   <si>
-    <t>Leaderboard</t>
-  </si>
-  <si>
     <t>Xếp hạng</t>
   </si>
   <si>
     <t>tut_mission</t>
   </si>
   <si>
-    <t>Could not connect to server</t>
-  </si>
-  <si>
-    <t>Could not share</t>
+    <t>LineBacker</t>
+  </si>
+  <si>
+    <t>Line Backer -- the best shoot them up game in 2014</t>
+  </si>
+  <si>
+    <t>Challenge your friends</t>
+  </si>
+  <si>
+    <t>I've got %d pts in Line Backer, follow me is %s. Kaka :v</t>
+  </si>
+  <si>
+    <t>Failed to share</t>
+  </si>
+  <si>
+    <t>Do not miss more than 3 B-52 bombers !!!</t>
+  </si>
+  <si>
+    <t>You do not have enough diamond!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to exit? </t>
+  </si>
+  <si>
+    <t>Connect  facebook for more friends, more gifts!</t>
+  </si>
+  <si>
+    <t>You have no gift. Invite your friends to play LineBacker to get more every day!</t>
+  </si>
+  <si>
+    <t>Failed to connect to server</t>
+  </si>
+  <si>
+    <t>%s is fighting to shoot down enemie planes in Line Backer. Come in to help your friend now!</t>
+  </si>
+  <si>
+    <t>You do not have enough live. Please wait !</t>
+  </si>
+  <si>
+    <t>Take off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Live in the legend of 12-days </t>
+  </si>
+  <si>
+    <t>1972 .... The enemy had attacked for several days mainly using the B-52 bomber at night ....</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>rate_msg</t>
+  </si>
+  <si>
+    <t>rate_rate</t>
+  </si>
+  <si>
+    <t>rate_no</t>
+  </si>
+  <si>
+    <t>rate_later</t>
+  </si>
+  <si>
+    <t>Bình chọn Điện Biên Phủ trên không 5 sao nhé!</t>
+  </si>
+  <si>
+    <t>Rate 5 stars for LineBacker!</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Remind me later</t>
+  </si>
+  <si>
+    <t>Để sau</t>
+  </si>
+  <si>
+    <t>Không, cảm ơn</t>
+  </si>
+  <si>
+    <t>No, thanks</t>
+  </si>
+  <si>
+    <t>game_package</t>
+  </si>
+  <si>
+    <t>com.chimgokien.phicongbutchi</t>
   </si>
 </sst>
 </file>
@@ -385,7 +427,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,6 +485,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCDACE6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6699"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -528,6 +582,9 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,6 +593,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF6699"/>
       <color rgb="FFCDACE6"/>
       <color rgb="FFB17ED8"/>
       <color rgb="FF25FF88"/>
@@ -816,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -827,7 +885,8 @@
     <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="46.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="92.5703125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -843,431 +902,486 @@
     </row>
     <row r="2" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>23</v>
+      <c r="A11" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>32</v>
+      <c r="A13" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>37</v>
+      <c r="A16" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="13" t="s">
-        <v>74</v>
-      </c>
       <c r="B29" s="1" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>109</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Language in menu
</commit_message>
<xml_diff>
--- a/trunk/Resources/language.xlsx
+++ b/trunk/Resources/language.xlsx
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -912,13 +912,13 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="11" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
+ replace background menu, start button menu
</commit_message>
<xml_diff>
--- a/trunk/Resources/language.xlsx
+++ b/trunk/Resources/language.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="130">
   <si>
     <t>Id</t>
   </si>
@@ -405,6 +405,15 @@
   </si>
   <si>
     <t>com.chimgokien.phicongbutchi</t>
+  </si>
+  <si>
+    <t>fb_logout_ask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to disconnect Facebook? </t>
+  </si>
+  <si>
+    <t>Bạn có muốn ngắt kết nối Facebook!</t>
   </si>
 </sst>
 </file>
@@ -874,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1088,299 +1097,310 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
+ Get boom immediately (GetBoomNow)
</commit_message>
<xml_diff>
--- a/trunk/Resources/language.xlsx
+++ b/trunk/Resources/language.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="131">
   <si>
     <t>Id</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Information</t>
   </si>
   <si>
-    <t>lose_error</t>
-  </si>
-  <si>
     <t>menu_thank_rate</t>
   </si>
   <si>
@@ -414,6 +411,12 @@
   </si>
   <si>
     <t>Bạn có muốn ngắt kết nối Facebook!</t>
+  </si>
+  <si>
+    <t>score_lack_diamond</t>
+  </si>
+  <si>
+    <t>lose_lack_diamond</t>
   </si>
 </sst>
 </file>
@@ -883,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -911,24 +914,24 @@
     </row>
     <row r="2" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>126</v>
-      </c>
       <c r="C3" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -936,7 +939,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -947,7 +950,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
@@ -958,7 +961,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -969,10 +972,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1013,7 +1016,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
@@ -1024,7 +1027,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>20</v>
@@ -1032,10 +1035,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
@@ -1054,10 +1057,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>24</v>
@@ -1076,18 +1079,18 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>28</v>
@@ -1098,84 +1101,84 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>28</v>
@@ -1186,211 +1189,211 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="1" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
+      <c r="B31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -1398,10 +1401,21 @@
         <v>116</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>123</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>